<commit_message>
หน้า Position ให้เพิ่ม ส่วนของ Advance Search และมี Parameter Position เป็น Auto Complete Search
</commit_message>
<xml_diff>
--- a/docroot/file/appraisal_position_template.xlsx
+++ b/docroot/file/appraisal_position_template.xlsx
@@ -72,12 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -144,7 +143,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -196,7 +195,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -398,30 +397,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
-    <col min="3" max="20" width="9.140625" style="2"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="24.85546875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="KEtOsoPrcjhtICzssnuVHVZiFk1kRiCpnrxw6amGF7PApi6Tx3TnbmU0gq6sz+YAC/t6HOQWHFyYPuWknoRHLg==" saltValue="1P/9AoWLOApbbBJp1PNWyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[Edited] : แก้หน้า import position เพิ่ม field job code
- download กรณีใน table ไม่มีข้อมูลให้ download template เปล่า โดยเพิ่ม
field job code
- download กรณีใน table มีข้อมูลให้ download ข้อมูลมาด้วย โดยเพิ่ม field
job code
- ผลจากการค้นหาที่หน้าเว็บตรง position list ให้เพิ่ม field Job Code
ต่อจาก Position Name
- หน้า Edit เพิ่ม field Position Code ต่อจาก Position Name
</commit_message>
<xml_diff>
--- a/docroot/file/appraisal_position_template.xlsx
+++ b/docroot/file/appraisal_position_template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GJ-Chokanan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC5F0276-D722-44F2-95C1-3EAFB9898D89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{1B4C7DB1-E634-44E8-956B-96089A25616F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,18 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
     <t>Position Code</t>
   </si>
   <si>
     <t>Position Name</t>
   </si>
+  <si>
+    <t>Job Code</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -47,9 +51,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,16 +76,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,32 +394,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4961FD86-5820-40B6-B644-1045F424F1E1}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KEtOsoPrcjhtICzssnuVHVZiFk1kRiCpnrxw6amGF7PApi6Tx3TnbmU0gq6sz+YAC/t6HOQWHFyYPuWknoRHLg==" saltValue="1P/9AoWLOApbbBJp1PNWyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>